<commit_message>
Changed files acording to first code review.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DariusDangi\Desktop\fwf-api-poc-performer\fwf-api-poc-performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818C5936-2B70-4EF7-B006-2AD8D074ED02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C3428F-1970-4C4D-912E-120C7FB794EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2070" yWindow="2505" windowWidth="23325" windowHeight="12480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="12852" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="88">
   <si>
     <t>Name</t>
   </si>
@@ -95,126 +95,206 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data.</t>
+  </si>
+  <si>
+    <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueFolder</t>
+  </si>
+  <si>
+    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>fwf-api-poc-performer</t>
+  </si>
+  <si>
+    <t>Api-POC</t>
+  </si>
+  <si>
+    <t>Api-POC-Queue</t>
+  </si>
+  <si>
+    <t>PathCatImage</t>
+  </si>
+  <si>
+    <t>C:\Users\DariusDangi\Desktop\Cat.jpg</t>
+  </si>
+  <si>
+    <t>PathDogImage</t>
+  </si>
+  <si>
+    <t>C:\Users\DariusDangi\Desktop\Dog.jpg</t>
+  </si>
+  <si>
+    <t>Path to saved cat image from API call. NOTE: change this acording to your case.</t>
+  </si>
+  <si>
+    <t>Path to saved dog image from API call. NOTE: change this acording to your case.</t>
+  </si>
+  <si>
+    <t>OutputReportPath</t>
+  </si>
+  <si>
+    <t>C:\Users\DariusDangi\Desktop\OutputReport.xlsx</t>
+  </si>
+  <si>
+    <t>Path to output report.</t>
+  </si>
+  <si>
+    <t>OutlookInputEmailAddress</t>
+  </si>
+  <si>
+    <t>darius.dangi@fwfcompany.com</t>
+  </si>
+  <si>
+    <t>Outlook email that is used to send mail messages.</t>
+  </si>
+  <si>
+    <t>SendImageMessage</t>
+  </si>
+  <si>
+    <t>You can find below images with your pet animals.</t>
+  </si>
+  <si>
+    <t>Message that it's written in the body of the mail that's sent.</t>
+  </si>
+  <si>
+    <t>ColumnOfInterest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animal </t>
+  </si>
+  <si>
+    <t>It will search in queue item for this specific content.</t>
+  </si>
+  <si>
+    <t>OutputReportSheetName</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>GetRowIndexColumnName</t>
+  </si>
+  <si>
+    <t>Searches for this specific column name to return the index of row.</t>
+  </si>
+  <si>
+    <t>OutputReportUpdatedColumn</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>This column value will be updated in the given dataTable.</t>
+  </si>
+  <si>
+    <t>OutlookInputAccount</t>
+  </si>
+  <si>
+    <t>This email address will be used to send the output report.</t>
+  </si>
+  <si>
+    <t>OutputReportSendTo</t>
+  </si>
+  <si>
+    <t>OutputReportSubject</t>
+  </si>
+  <si>
+    <t>OutputReportBody</t>
+  </si>
+  <si>
+    <t>Output Report</t>
+  </si>
+  <si>
+    <t>You have attached below the output report.</t>
+  </si>
+  <si>
+    <t>EndpointDogAPI</t>
+  </si>
+  <si>
+    <t>EndpointCatAPI</t>
+  </si>
+  <si>
+    <t>https://dog.ceo/api/breeds/image/random</t>
+  </si>
+  <si>
+    <t>It is used to get a random picture of dogs.</t>
+  </si>
+  <si>
+    <t>https://api.thecatapi.com/v1/images/search</t>
+  </si>
+  <si>
+    <t>It is used to get a random picture of cats.</t>
+  </si>
+  <si>
+    <t>GetAnimalFail</t>
+  </si>
+  <si>
+    <t>Failed to get success status from API call.</t>
+  </si>
+  <si>
+    <t>GetAnimalDownloadFail</t>
+  </si>
+  <si>
+    <t>Failed to download animal picture from API call.</t>
+  </si>
+  <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with business exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data.</t>
-  </si>
-  <si>
-    <t>OrchestratorAssetFolder</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueFolder</t>
-  </si>
-  <si>
-    <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
-  </si>
-  <si>
-    <t>MaxConsecutiveSystemExceptions</t>
-  </si>
-  <si>
-    <t>ExceptionMessage_ConsecutiveErrors</t>
-  </si>
-  <si>
-    <t>RetryNumberGetTransactionItem</t>
-  </si>
-  <si>
-    <t>RetryNumberSetTransactionStatus</t>
-  </si>
-  <si>
-    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
-  </si>
-  <si>
-    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
-  </si>
-  <si>
-    <t>ShouldMarkJobAsFaulted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
-  </si>
-  <si>
-    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
-  </si>
-  <si>
-    <t>fwf-api-poc-performer</t>
-  </si>
-  <si>
-    <t>Api-POC</t>
-  </si>
-  <si>
-    <t>Api-POC-Queue</t>
-  </si>
-  <si>
-    <t>PathCatImage</t>
-  </si>
-  <si>
-    <t>C:\Users\DariusDangi\Desktop\Cat.jpg</t>
-  </si>
-  <si>
-    <t>PathDogImage</t>
-  </si>
-  <si>
-    <t>C:\Users\DariusDangi\Desktop\Dog.jpg</t>
-  </si>
-  <si>
-    <t>Path to saved cat image from API call. NOTE: change this acording to your case.</t>
-  </si>
-  <si>
-    <t>Path to saved dog image from API call. NOTE: change this acording to your case.</t>
-  </si>
-  <si>
-    <t>OutputReportPath</t>
-  </si>
-  <si>
-    <t>C:\Users\DariusDangi\Desktop\OutputReport.xlsx</t>
-  </si>
-  <si>
-    <t>Path to output report.</t>
-  </si>
-  <si>
-    <t>OutlookInputEmailAddress</t>
-  </si>
-  <si>
-    <t>darius.dangi@fwfcompany.com</t>
-  </si>
-  <si>
-    <t>Outlook email that is used to send mail messages.</t>
-  </si>
-  <si>
-    <t>SendImageMessage</t>
-  </si>
-  <si>
-    <t>You can find below images with your pet animals.</t>
-  </si>
-  <si>
-    <t>Message that it's written in the body of the mail that's sent.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -238,12 +318,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,11 +336,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -276,10 +349,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -595,7 +666,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -642,10 +713,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>21</v>
@@ -653,13 +724,13 @@
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -668,7 +739,7 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>22</v>
@@ -677,80 +748,182 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
         <v>46</v>
       </c>
-      <c r="B7" t="s">
-        <v>47</v>
-      </c>
       <c r="C7" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
         <v>52</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
-        <v>57</v>
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
         <v>58</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>70</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>85</v>
+      </c>
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+    </row>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1719,11 +1892,8 @@
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{172B33C1-1065-4F98-9FDE-3BDA0C52839E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1785,18 +1955,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1820,7 +1990,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1842,7 +2012,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1853,7 +2023,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1864,53 +2034,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2912,7 +3082,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>